<commit_message>
Put all outputs to one directory. Fix minor bugs
</commit_message>
<xml_diff>
--- a/TrackCreate.xlsx
+++ b/TrackCreate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">num_files_per_group</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">list</t>
   </si>
   <si>
-    <t xml:space="preserve">type (Overview)</t>
+    <t xml:space="preserve">type</t>
   </si>
   <si>
     <t xml:space="preserve">reviewglossika.py</t>
@@ -52,55 +52,33 @@
     <t xml:space="preserve">-m</t>
   </si>
   <si>
-    <t xml:space="preserve">glossikatest</t>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-15 1-3 16-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixaccent.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accenttest</t>
   </si>
   <si>
     <t xml:space="preserve">all</t>
   </si>
   <si>
-    <t xml:space="preserve">4-15 1-3 16-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mixaccent.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accenttest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group</t>
-  </si>
-  <si>
     <t xml:space="preserve">7 6 10 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mixgrammar.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grammartest1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grammartest2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overviewglossika.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23-45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -168,12 +146,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -194,10 +168,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -255,13 +229,13 @@
       <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -291,77 +265,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>